<commit_message>
Adds to scale rotations and also a help menu.
</commit_message>
<xml_diff>
--- a/planet-stats.xlsx
+++ b/planet-stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Rotation</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>scaled value</t>
+  </si>
+  <si>
+    <t>Revolution in Earth Days</t>
   </si>
 </sst>
 </file>
@@ -139,8 +142,8 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -179,11 +182,11 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P18"/>
+  <dimension ref="B2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="163" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="136" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,23 +477,24 @@
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="H2" s="8" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
       <c r="K2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -522,19 +526,22 @@
         <v>17</v>
       </c>
       <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -567,15 +574,16 @@
       <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4"/>
+      <c r="N4" s="2">
         <v>7.5</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -590,7 +598,7 @@
         <f t="shared" ref="E5:E14" si="0">D5*2</f>
         <v>7.0145177519045565E-3</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>3200</v>
       </c>
       <c r="G5" s="5">
@@ -613,17 +621,21 @@
       <c r="L5" s="4">
         <v>0.24</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
+        <f>L5*365</f>
+        <v>87.6</v>
+      </c>
+      <c r="N5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>7</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -638,7 +650,7 @@
         <f t="shared" si="0"/>
         <v>1.7392554261894493E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>3200</v>
       </c>
       <c r="G6" s="5">
@@ -661,17 +673,21 @@
       <c r="L6" s="4">
         <v>0.62</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
+        <f t="shared" ref="M6:M13" si="2">L6*365</f>
+        <v>226.3</v>
+      </c>
+      <c r="N6" s="2">
         <v>178</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>3.39</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -686,7 +702,7 @@
         <f t="shared" si="0"/>
         <v>1.8341239039816014E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>3200</v>
       </c>
       <c r="G7" s="5">
@@ -708,17 +724,21 @@
       <c r="L7" s="4">
         <v>1</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="N7" s="2">
         <v>23.4</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>0</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -733,7 +753,7 @@
         <f t="shared" si="0"/>
         <v>9.7743280149489714E-3</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>3200</v>
       </c>
       <c r="G8" s="5">
@@ -756,17 +776,21 @@
       <c r="L8" s="4">
         <v>0.94</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="4">
+        <f t="shared" si="2"/>
+        <v>343.09999999999997</v>
+      </c>
+      <c r="N8" s="2">
         <v>25</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>1.85</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -781,7 +805,7 @@
         <f t="shared" si="0"/>
         <v>0.20554836854966221</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>3200</v>
       </c>
       <c r="G9" s="5">
@@ -804,20 +828,24 @@
       <c r="L9" s="4">
         <v>11.86</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="4">
+        <f t="shared" si="2"/>
+        <v>4328.8999999999996</v>
+      </c>
+      <c r="N9" s="2">
         <v>3.08</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>1.3</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -832,7 +860,7 @@
         <f t="shared" si="0"/>
         <v>0.17326433807675723</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>3200</v>
       </c>
       <c r="G10" s="5">
@@ -855,20 +883,24 @@
       <c r="L10" s="4">
         <v>29.46</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="4">
+        <f t="shared" si="2"/>
+        <v>10752.9</v>
+      </c>
+      <c r="N10" s="2">
         <v>26.7</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>2.46</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -883,7 +915,7 @@
         <f t="shared" si="0"/>
         <v>7.4744861290786252E-2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>3200</v>
       </c>
       <c r="G11" s="5">
@@ -906,20 +938,24 @@
       <c r="L11" s="4">
         <v>30685</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="4">
+        <f t="shared" si="2"/>
+        <v>11200025</v>
+      </c>
+      <c r="N11" s="2">
         <v>97.9</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>0.77</v>
       </c>
-      <c r="O11" s="3">
+      <c r="P11" s="3">
         <v>4.7E-2</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -934,7 +970,7 @@
         <f t="shared" si="0"/>
         <v>7.1180106367687221E-2</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>3200</v>
       </c>
       <c r="G12" s="5">
@@ -957,20 +993,24 @@
       <c r="L12" s="4">
         <v>60190</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
+        <f t="shared" si="2"/>
+        <v>21969350</v>
+      </c>
+      <c r="N12" s="2">
         <v>29.6</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>1.77</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -985,7 +1025,7 @@
         <f t="shared" si="0"/>
         <v>3.4497628288055198E-3</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>3200</v>
       </c>
       <c r="G13" s="5">
@@ -1008,17 +1048,21 @@
       <c r="L13" s="4">
         <v>247.92</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="4">
+        <f t="shared" si="2"/>
+        <v>90490.799999999988</v>
+      </c>
+      <c r="N13" s="2">
         <v>122.5</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>17.149999999999999</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P13" s="3">
         <v>0.248</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1033,7 +1077,7 @@
         <f t="shared" si="0"/>
         <v>5.0021561017680035E-3</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>3200</v>
       </c>
       <c r="G14" s="5">
@@ -1056,17 +1100,20 @@
       <c r="L14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="4">
+        <v>27.32</v>
+      </c>
+      <c r="N14" s="2">
         <v>6.68</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>5.14</v>
       </c>
-      <c r="O14" s="3">
+      <c r="P14" s="3">
         <v>5.4899999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="H16" s="6">
         <f>384400/H7</f>
         <v>2.5695549582952005E-3</v>
@@ -1076,16 +1123,38 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="L17">
         <f>L16/365</f>
         <v>0.24109589041095891</v>
       </c>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="H18">
         <f>E4*H7/C4</f>
         <v>430.06436682478079</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <v>6380</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1740</v>
+      </c>
+      <c r="F19">
+        <v>384400</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>1.8</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+      <c r="F20">
+        <v>110.459770115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes the speeds of the planets and zooming to the center.
</commit_message>
<xml_diff>
--- a/planet-stats.xlsx
+++ b/planet-stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="2060" yWindow="2280" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,20 +466,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="136" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="150" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="5" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="7" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -622,8 +621,7 @@
         <v>0.24</v>
       </c>
       <c r="M5" s="4">
-        <f>L5*365</f>
-        <v>87.6</v>
+        <v>88</v>
       </c>
       <c r="N5" s="2">
         <v>0</v>
@@ -674,8 +672,7 @@
         <v>0.62</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6:M13" si="2">L6*365</f>
-        <v>226.3</v>
+        <v>224.7</v>
       </c>
       <c r="N6" s="2">
         <v>178</v>
@@ -725,8 +722,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="2"/>
-        <v>365</v>
+        <v>365.2</v>
       </c>
       <c r="N7" s="2">
         <v>23.4</v>
@@ -777,8 +773,7 @@
         <v>0.94</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="2"/>
-        <v>343.09999999999997</v>
+        <v>687</v>
       </c>
       <c r="N8" s="2">
         <v>25</v>
@@ -829,8 +824,7 @@
         <v>11.86</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="2"/>
-        <v>4328.8999999999996</v>
+        <v>4331</v>
       </c>
       <c r="N9" s="2">
         <v>3.08</v>
@@ -884,8 +878,7 @@
         <v>29.46</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="2"/>
-        <v>10752.9</v>
+        <v>10747</v>
       </c>
       <c r="N10" s="2">
         <v>26.7</v>
@@ -939,8 +932,7 @@
         <v>30685</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="2"/>
-        <v>11200025</v>
+        <v>30589</v>
       </c>
       <c r="N11" s="2">
         <v>97.9</v>
@@ -994,8 +986,7 @@
         <v>60190</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="2"/>
-        <v>21969350</v>
+        <v>59800</v>
       </c>
       <c r="N12" s="2">
         <v>29.6</v>
@@ -1049,8 +1040,7 @@
         <v>247.92</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="2"/>
-        <v>90490.799999999988</v>
+        <v>90560</v>
       </c>
       <c r="N13" s="2">
         <v>122.5</v>

</xml_diff>

<commit_message>
Adds labels, fixes zooming, positions correctly.
</commit_message>
<xml_diff>
--- a/planet-stats.xlsx
+++ b/planet-stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="2280" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1500" yWindow="9240" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Rotation</t>
   </si>
@@ -132,18 +132,52 @@
   </si>
   <si>
     <t>Revolution in Earth Days</t>
+  </si>
+  <si>
+    <t>Saturn D Ring</t>
+  </si>
+  <si>
+    <t>Saturn C Ring</t>
+  </si>
+  <si>
+    <t>Saturn B Ring</t>
+  </si>
+  <si>
+    <t>Saturn A Ring</t>
+  </si>
+  <si>
+    <t>Saturn F Ring</t>
+  </si>
+  <si>
+    <t>Outer Radius</t>
+  </si>
+  <si>
+    <t>Inner Radius</t>
+  </si>
+  <si>
+    <t>Outer Scaled</t>
+  </si>
+  <si>
+    <t>Inner Scaled</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Width Scaled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="169" formatCode="0.000;[Red]0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -174,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -187,6 +221,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,18 +501,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q20"/>
+  <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="7" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
     <col min="12" max="13" width="23.33203125" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
@@ -1104,47 +1142,212 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="H16" s="6">
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>66900</v>
+      </c>
+      <c r="D17">
+        <v>74510</v>
+      </c>
+      <c r="E17">
+        <v>7500</v>
+      </c>
+      <c r="F17" s="10">
+        <f>C17/I17*2</f>
+        <v>0.19232427770590771</v>
+      </c>
+      <c r="G17" s="10">
+        <f>D17/I17*2</f>
+        <v>0.21420152364524939</v>
+      </c>
+      <c r="H17" s="10">
+        <f>E17/I17*2</f>
+        <v>2.1561017680034499E-2</v>
+      </c>
+      <c r="I17" s="12">
+        <v>695700</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1">
+        <v>74658</v>
+      </c>
+      <c r="D18">
+        <v>92000</v>
+      </c>
+      <c r="E18">
+        <v>17500</v>
+      </c>
+      <c r="F18" s="10">
+        <f>C18/I18*2</f>
+        <v>0.21462699439413541</v>
+      </c>
+      <c r="G18" s="10">
+        <f>D18/I18*2</f>
+        <v>0.26448181687508981</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" ref="H18:H21" si="2">E18/I18*2</f>
+        <v>5.030904125341383E-2</v>
+      </c>
+      <c r="I18" s="12">
+        <v>695700</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1">
+        <v>92000</v>
+      </c>
+      <c r="D19">
+        <v>117580</v>
+      </c>
+      <c r="E19">
+        <v>25500</v>
+      </c>
+      <c r="F19" s="10">
+        <f>C19/I19*2</f>
+        <v>0.26448181687508981</v>
+      </c>
+      <c r="G19" s="10">
+        <f>D19/I19*2</f>
+        <v>0.33801926117579417</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="2"/>
+        <v>7.3307460112117293E-2</v>
+      </c>
+      <c r="I19" s="12">
+        <v>695700</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1">
+        <v>122170</v>
+      </c>
+      <c r="D20">
+        <v>139380</v>
+      </c>
+      <c r="E20">
+        <v>14600</v>
+      </c>
+      <c r="F20" s="10">
+        <f>C20/I20*2</f>
+        <v>0.35121460399597526</v>
+      </c>
+      <c r="G20" s="10">
+        <f>D20/I20*2</f>
+        <v>0.40068995256576112</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="2"/>
+        <v>4.1972114417133825E-2</v>
+      </c>
+      <c r="I20" s="12">
+        <v>695700</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1">
+        <v>140180</v>
+      </c>
+      <c r="D21" s="1">
+        <v>154000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>500</v>
+      </c>
+      <c r="F21" s="10">
+        <f>C21/I21*2</f>
+        <v>0.40298979445163147</v>
+      </c>
+      <c r="G21" s="10">
+        <f>D21/I21*2</f>
+        <v>0.44271956303004167</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="2"/>
+        <v>1.4374011786689666E-3</v>
+      </c>
+      <c r="I21" s="12">
+        <v>695700</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I22" s="11"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="1">
+        <v>6380</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1740</v>
+      </c>
+      <c r="F25">
+        <v>384400</v>
+      </c>
+      <c r="H25" s="6">
         <f>384400/H7</f>
         <v>2.5695549582952005E-3</v>
       </c>
-      <c r="L16">
+      <c r="L25">
         <f>88</f>
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="L17">
-        <f>L16/365</f>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>1.8</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <v>110.459770115</v>
+      </c>
+      <c r="L26">
+        <f>L25/365</f>
         <v>0.24109589041095891</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="H18">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H27">
         <f>E4*H7/C4</f>
         <v>430.06436682478079</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C19" s="1">
-        <v>6380</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1740</v>
-      </c>
-      <c r="F19">
-        <v>384400</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C20">
-        <v>1.8</v>
-      </c>
-      <c r="E20">
-        <v>0.5</v>
-      </c>
-      <c r="F20">
-        <v>110.459770115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>